<commit_message>
Formel Usecase 5 Visionsdokument Tidsregistrering - NO
</commit_message>
<xml_diff>
--- a/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering i PTE projektet - Nada Omer.xlsx
+++ b/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering i PTE projektet - Nada Omer.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nada\Desktop\Datamatiker\Systemudvikling\PTE projekt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nada\git\PTE-projekt\Documentation\08 - Project Management\Tidsregistrering\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="73">
   <si>
     <t>Business-Process Analyst</t>
   </si>
@@ -201,9 +201,6 @@
     <t>NO</t>
   </si>
   <si>
-    <t>System analyst</t>
-  </si>
-  <si>
     <t>1 time :  30 min.</t>
   </si>
   <si>
@@ -235,6 +232,24 @@
   </si>
   <si>
     <t>Git Hub opsætning.</t>
+  </si>
+  <si>
+    <t>1 time : 00</t>
+  </si>
+  <si>
+    <t>1 time : 45 min.</t>
+  </si>
+  <si>
+    <t>Visionsdokument + FURPS</t>
+  </si>
+  <si>
+    <t>Formel Use case 5 + Domæne model for UC 5</t>
+  </si>
+  <si>
+    <t>Iterationsplan</t>
+  </si>
+  <si>
+    <t>2 time : 50</t>
   </si>
 </sst>
 </file>
@@ -288,9 +303,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -303,6 +315,9 @@
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -618,36 +633,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="48.140625" customWidth="1"/>
     <col min="9" max="9" width="24.5703125" customWidth="1"/>
     <col min="11" max="11" width="31.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
@@ -683,217 +698,332 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
+    <row r="4" spans="1:11" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
         <v>42800</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="C4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" s="9">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="H4" s="9">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>42800</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G5" s="9">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H5" s="9">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>42800</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G6" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="H6" s="9">
+        <v>0.53125</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>42800</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G7" s="9">
+        <v>0.53125</v>
+      </c>
+      <c r="H7" s="9">
+        <v>0.53472222222222221</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>42800</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="G4" s="10">
-        <v>0.35416666666666669</v>
-      </c>
-      <c r="H4" s="10">
-        <v>0.40972222222222227</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
+      <c r="G8" s="5">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="H8" s="5">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
         <v>42800</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="G5" s="10">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="H5" s="10">
+      <c r="C9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="H9" s="5">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>42801</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" s="5">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="H10" s="5">
+        <v>0.4375</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>42801</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" s="5">
+        <v>0.4375</v>
+      </c>
+      <c r="H11" s="5">
         <v>0.47916666666666669</v>
       </c>
-      <c r="I5" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
-        <v>42800</v>
-      </c>
-      <c r="B6" s="8" t="s">
+      <c r="I11" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>42801</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="G6" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="H6" s="10">
-        <v>0.53125</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
-        <v>42800</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="G7" s="10">
-        <v>0.53125</v>
-      </c>
-      <c r="H7" s="10">
-        <v>0.53472222222222221</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
-        <v>42800</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="G8" s="6">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="H8" s="6">
-        <v>0.57291666666666663</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
-        <v>42800</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" s="8"/>
-      <c r="F9" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="G9" s="6">
-        <v>0.60416666666666663</v>
-      </c>
-      <c r="H9" s="6">
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
-        <v>42801</v>
-      </c>
-      <c r="B10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="8"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
+      <c r="C12" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="G12" s="5">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="H12" s="5">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
         <v>42802</v>
       </c>
-      <c r="K11" s="2"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
+      <c r="B13" s="7"/>
+      <c r="C13" s="4"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="7"/>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
         <v>42803</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
+      <c r="C14" s="4"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
         <v>42804</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
+      <c r="C15" s="4"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C16" s="4"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C17" s="4"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C18" s="4"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C19" s="4"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C20" s="4"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C21" s="4"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C22" s="4"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C23" s="4"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C24" s="4"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C25" s="4"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C26" s="4"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
+      <c r="C27" s="4"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="C28" s="4"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E107">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E109">
       <formula1>GyldigeRoller</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C28">
       <formula1>Deltagere</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
OC 4 - beregnTvaertkraft er lavet
</commit_message>
<xml_diff>
--- a/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering i PTE projektet - Nada Omer.xlsx
+++ b/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering i PTE projektet - Nada Omer.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="81">
   <si>
     <t>Business-Process Analyst</t>
   </si>
@@ -234,9 +234,6 @@
     <t>Git Hub opsætning.</t>
   </si>
   <si>
-    <t>1 time : 00</t>
-  </si>
-  <si>
     <t>1 time : 45 min.</t>
   </si>
   <si>
@@ -249,22 +246,34 @@
     <t>Iterationsplan</t>
   </si>
   <si>
-    <t>2 time : 50</t>
-  </si>
-  <si>
     <t>Usability gools</t>
   </si>
   <si>
-    <t>0 time : 30</t>
-  </si>
-  <si>
     <t>SSD for Usecase 2</t>
   </si>
   <si>
-    <t>0 time : 20</t>
-  </si>
-  <si>
-    <t>FURSP</t>
+    <t>FURPS</t>
+  </si>
+  <si>
+    <t>Skabelon til OC</t>
+  </si>
+  <si>
+    <t>0 time : 30 min.</t>
+  </si>
+  <si>
+    <t>2 time : 50 min.</t>
+  </si>
+  <si>
+    <t>0 time : 20 min.</t>
+  </si>
+  <si>
+    <t>OC1 for angivVaegt</t>
+  </si>
+  <si>
+    <t>1 time : 15 min.</t>
+  </si>
+  <si>
+    <t>OC3 for beregnNormalkraft</t>
   </si>
 </sst>
 </file>
@@ -648,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -886,7 +895,7 @@
         <v>3</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G10" s="5">
         <v>0.36458333333333331</v>
@@ -895,7 +904,7 @@
         <v>0.4375</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -912,7 +921,7 @@
         <v>3</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G11" s="5">
         <v>0.4375</v>
@@ -921,7 +930,7 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K11" s="2"/>
     </row>
@@ -939,7 +948,7 @@
         <v>11</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G12" s="5">
         <v>0.52083333333333337</v>
@@ -948,7 +957,7 @@
         <v>0.63888888888888895</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="K12" s="2"/>
     </row>
@@ -966,7 +975,7 @@
         <v>3</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G13" s="5">
         <v>0.34027777777777773</v>
@@ -975,7 +984,7 @@
         <v>0.3611111111111111</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="K13" s="2"/>
     </row>
@@ -993,7 +1002,7 @@
         <v>3</v>
       </c>
       <c r="F14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G14" s="5">
         <v>0.3611111111111111</v>
@@ -1002,7 +1011,7 @@
         <v>0.38194444444444442</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="K14" s="2"/>
     </row>
@@ -1020,7 +1029,7 @@
         <v>3</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G15" s="5">
         <v>0.40625</v>
@@ -1029,7 +1038,7 @@
         <v>0.4201388888888889</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="K15" s="2"/>
     </row>
@@ -1043,88 +1052,153 @@
       <c r="C16" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="8"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="7"/>
+      <c r="E16" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G16" s="5">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="H16" s="5">
+        <v>0.54866898148148147</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>62</v>
+      </c>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
+        <v>42802</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="G17" s="5">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="H17" s="5">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>42802</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="G18" s="5">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="H18" s="5">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
         <v>42803</v>
       </c>
-      <c r="C17" s="4"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
+      <c r="C19" s="4"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
         <v>42804</v>
       </c>
-      <c r="C18" s="4"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="C19" s="4"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="C21" s="4"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="C23" s="4"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="C24" s="4"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="C25" s="4"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="C26" s="4"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="C27" s="4"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="C28" s="4"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="C29" s="4"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="C30" s="4"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="C31" s="4"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
+      <c r="C32" s="4"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="C33" s="4"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E112">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E114">
       <formula1>GyldigeRoller</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C33">
       <formula1>Deltagere</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Har lavet SD og DCD til OC1
</commit_message>
<xml_diff>
--- a/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering i PTE projektet - Nada Omer.xlsx
+++ b/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering i PTE projektet - Nada Omer.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="93">
   <si>
     <t>Business-Process Analyst</t>
   </si>
@@ -274,6 +274,42 @@
   </si>
   <si>
     <t>OC3 for beregnNormalkraft</t>
+  </si>
+  <si>
+    <t>Sekvens og klasse diagram</t>
+  </si>
+  <si>
+    <t>OC4</t>
+  </si>
+  <si>
+    <t>DMU 4. semster</t>
+  </si>
+  <si>
+    <t>2 time : 25 min.</t>
+  </si>
+  <si>
+    <t>0 time : 10 min.</t>
+  </si>
+  <si>
+    <t>1 time : 10 min.</t>
+  </si>
+  <si>
+    <t>SD2 og KD for OC2</t>
+  </si>
+  <si>
+    <t>SD3</t>
+  </si>
+  <si>
+    <t>OC2</t>
+  </si>
+  <si>
+    <t>0 time : 35 min.</t>
+  </si>
+  <si>
+    <t>SD4 for OC4</t>
+  </si>
+  <si>
+    <t>TestCase for OC1</t>
   </si>
 </sst>
 </file>
@@ -657,10 +693,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1127,78 +1163,295 @@
       <c r="A19" s="6">
         <v>42803</v>
       </c>
+      <c r="B19" s="7"/>
       <c r="C19" s="4"/>
+      <c r="F19" s="8"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>42804</v>
       </c>
-      <c r="C20" s="4"/>
+      <c r="B20" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="G20" s="5">
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="H20" s="5">
+        <v>0.4375</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="C21" s="4"/>
+      <c r="A21" s="6">
+        <v>42804</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G21" s="5">
+        <v>0.4375</v>
+      </c>
+      <c r="H21" s="5">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="C22" s="4"/>
+      <c r="A22" s="6">
+        <v>42804</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="G22" s="5">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="H22" s="5">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="C23" s="4"/>
+      <c r="A23" s="6">
+        <v>42804</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" t="s">
+        <v>5</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="G23" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="H23" s="5">
+        <v>0.54861111111111105</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
+      <c r="A24" s="6">
+        <v>42805</v>
+      </c>
       <c r="C24" s="4"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
+      <c r="A25" s="6">
+        <v>42806</v>
+      </c>
       <c r="C25" s="4"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="C26" s="4"/>
+      <c r="A26" s="6">
+        <v>42807</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" t="s">
+        <v>5</v>
+      </c>
+      <c r="F26" t="s">
+        <v>87</v>
+      </c>
+      <c r="G26" s="5">
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="H26" s="5">
+        <v>0.37847222222222227</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="C27" s="4"/>
+      <c r="A27" s="6">
+        <v>42807</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="7"/>
+      <c r="E27" t="s">
+        <v>26</v>
+      </c>
+      <c r="F27" t="s">
+        <v>88</v>
+      </c>
+      <c r="G27" s="5">
+        <v>0.38194444444444442</v>
+      </c>
+      <c r="H27" s="5">
+        <v>0.40625</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="C28" s="4"/>
+      <c r="A28" s="6">
+        <v>42807</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" t="s">
+        <v>26</v>
+      </c>
+      <c r="F28" t="s">
+        <v>89</v>
+      </c>
+      <c r="G28" s="5">
+        <v>0.40625</v>
+      </c>
+      <c r="H28" s="5">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="C29" s="4"/>
+      <c r="A29" s="6">
+        <v>42807</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E29" t="s">
+        <v>5</v>
+      </c>
+      <c r="F29" t="s">
+        <v>91</v>
+      </c>
+      <c r="G29" s="5">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H29" s="5">
+        <v>0.4375</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="C30" s="4"/>
+      <c r="A30" s="6">
+        <v>42807</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30" t="s">
+        <v>26</v>
+      </c>
+      <c r="F30" t="s">
+        <v>92</v>
+      </c>
+      <c r="G30" s="5">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="H30" s="5">
+        <v>0.46527777777777773</v>
+      </c>
+      <c r="I30" s="7" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
+      <c r="A31" s="6">
+        <v>42808</v>
+      </c>
       <c r="C31" s="4"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
+      <c r="A32" s="6">
+        <v>42809</v>
+      </c>
       <c r="C32" s="4"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
+      <c r="A33" s="6">
+        <v>42810</v>
+      </c>
       <c r="C33" s="4"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
+      <c r="C34" s="4"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+      <c r="C35" s="4"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E114">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E116">
       <formula1>GyldigeRoller</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C33">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C35">
       <formula1>Deltagere</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Tidsregistrering, fordi Anders sagde at vi skal gøre det.
</commit_message>
<xml_diff>
--- a/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering i PTE projektet - Nada Omer.xlsx
+++ b/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering i PTE projektet - Nada Omer.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="107">
   <si>
     <t>Business-Process Analyst</t>
   </si>
@@ -310,6 +310,48 @@
   </si>
   <si>
     <t>TestCase for OC1</t>
+  </si>
+  <si>
+    <t>SD og DCD for OC1</t>
+  </si>
+  <si>
+    <t>SD og DCD for OC2</t>
+  </si>
+  <si>
+    <t>1 time : 30 min.</t>
+  </si>
+  <si>
+    <t>0 time :30 min.</t>
+  </si>
+  <si>
+    <t>AD, DD og TC for UC7</t>
+  </si>
+  <si>
+    <t>UC, DOM og TC for UC8</t>
+  </si>
+  <si>
+    <t>1 time : 25 min.</t>
+  </si>
+  <si>
+    <t>Implementerer OC4</t>
+  </si>
+  <si>
+    <t>Krydstjeck for UC7</t>
+  </si>
+  <si>
+    <t>Krydstjeck for UC8</t>
+  </si>
+  <si>
+    <t>Review kode til OC3</t>
+  </si>
+  <si>
+    <t>Review kode til OC1</t>
+  </si>
+  <si>
+    <t>Review kode til OC2</t>
+  </si>
+  <si>
+    <t>0 time : 15 min.</t>
   </si>
 </sst>
 </file>
@@ -353,9 +395,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -693,10 +734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,327 +752,327 @@
     <col min="11" max="11" width="31.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+    <row r="4" spans="1:11" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
         <v>42800</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4" s="7" t="s">
+      <c r="B4" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="8">
         <v>0.35416666666666669</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="8">
         <v>0.40972222222222227</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+    <row r="5" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
         <v>42800</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" s="7" t="s">
+      <c r="B5" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="8">
         <v>0.41666666666666669</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="8">
         <v>0.47916666666666669</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+    <row r="6" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
         <v>42800</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" s="7" t="s">
+      <c r="B6" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="8">
         <v>0.5</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="8">
         <v>0.53125</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+    <row r="7" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
         <v>42800</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" s="7" t="s">
+      <c r="B7" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="8">
         <v>0.53125</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7" s="8">
         <v>0.53472222222222221</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="6" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+      <c r="A8" s="5">
         <v>42800</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7" t="s">
+      <c r="B8" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="4">
         <v>0.54166666666666663</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="4">
         <v>0.57291666666666663</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="I8" s="6" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
+      <c r="A9" s="5">
         <v>42800</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7" t="s">
+      <c r="B9" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="4">
         <v>0.60416666666666663</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="4">
         <v>0.64583333333333337</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="I9" s="6" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
+      <c r="A10" s="5">
         <v>42801</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="7"/>
+      <c r="B10" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="6"/>
       <c r="E10" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="4">
         <v>0.36458333333333331</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="4">
         <v>0.4375</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="I10" s="6" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
+      <c r="A11" s="5">
         <v>42801</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11" s="4" t="s">
+      <c r="B11" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>43</v>
       </c>
       <c r="E11" t="s">
         <v>3</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="4">
         <v>0.4375</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="4">
         <v>0.47916666666666669</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="I11" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="K11" s="2"/>
+      <c r="K11" s="1"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
+      <c r="A12" s="5">
         <v>42801</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" s="4" t="s">
+      <c r="B12" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>43</v>
       </c>
       <c r="E12" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="4">
         <v>0.52083333333333337</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H12" s="4">
         <v>0.63888888888888895</v>
       </c>
-      <c r="I12" s="7" t="s">
+      <c r="I12" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="K12" s="2"/>
+      <c r="K12" s="1"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
+      <c r="A13" s="5">
         <v>42802</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" s="4" t="s">
+      <c r="B13" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>43</v>
       </c>
       <c r="E13" t="s">
         <v>3</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="4">
         <v>0.34027777777777773</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H13" s="4">
         <v>0.3611111111111111</v>
       </c>
-      <c r="I13" s="7" t="s">
+      <c r="I13" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="K13" s="2"/>
+      <c r="K13" s="1"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
+      <c r="A14" s="5">
         <v>42802</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" s="4" t="s">
+      <c r="B14" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>43</v>
       </c>
       <c r="E14" t="s">
@@ -1040,257 +1081,257 @@
       <c r="F14" t="s">
         <v>71</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="4">
         <v>0.3611111111111111</v>
       </c>
-      <c r="H14" s="5">
+      <c r="H14" s="4">
         <v>0.38194444444444442</v>
       </c>
-      <c r="I14" s="7" t="s">
+      <c r="I14" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="K14" s="2"/>
+      <c r="K14" s="1"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
+      <c r="A15" s="5">
         <v>42802</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="4" t="s">
+      <c r="B15" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>43</v>
       </c>
       <c r="E15" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15" s="4">
         <v>0.40625</v>
       </c>
-      <c r="H15" s="5">
+      <c r="H15" s="4">
         <v>0.4201388888888889</v>
       </c>
-      <c r="I15" s="7" t="s">
+      <c r="I15" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="K15" s="2"/>
+      <c r="K15" s="1"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="6">
+      <c r="A16" s="5">
         <v>42802</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" s="4" t="s">
+      <c r="B16" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>43</v>
       </c>
       <c r="E16" t="s">
         <v>3</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F16" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G16" s="4">
         <v>0.54166666666666663</v>
       </c>
-      <c r="H16" s="5">
+      <c r="H16" s="4">
         <v>0.54866898148148147</v>
       </c>
-      <c r="I16" s="7" t="s">
+      <c r="I16" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="K16" s="2"/>
+      <c r="K16" s="1"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
+      <c r="A17" s="5">
         <v>42802</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C17" s="4" t="s">
+      <c r="B17" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>43</v>
       </c>
       <c r="E17" t="s">
         <v>3</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F17" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="G17" s="5">
+      <c r="G17" s="4">
         <v>0.55208333333333337</v>
       </c>
-      <c r="H17" s="5">
+      <c r="H17" s="4">
         <v>0.57291666666666663</v>
       </c>
-      <c r="I17" s="7" t="s">
+      <c r="I17" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="K17" s="2"/>
+      <c r="K17" s="1"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
+      <c r="A18" s="5">
         <v>42802</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18" s="4" t="s">
+      <c r="B18" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>43</v>
       </c>
       <c r="E18" t="s">
         <v>3</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F18" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G18" s="4">
         <v>0.57638888888888895</v>
       </c>
-      <c r="H18" s="5">
+      <c r="H18" s="4">
         <v>0.62847222222222221</v>
       </c>
-      <c r="I18" s="7" t="s">
+      <c r="I18" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="K18" s="2"/>
+      <c r="K18" s="1"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="6">
+      <c r="A19" s="5">
         <v>42803</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="4"/>
-      <c r="F19" s="8"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="3"/>
+      <c r="F19" s="7"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="6">
+      <c r="A20" s="5">
         <v>42804</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="4" t="s">
+      <c r="B20" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>43</v>
       </c>
       <c r="E20" t="s">
         <v>5</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F20" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="G20" s="5">
+      <c r="G20" s="4">
         <v>0.33680555555555558</v>
       </c>
-      <c r="H20" s="5">
+      <c r="H20" s="4">
         <v>0.4375</v>
       </c>
-      <c r="I20" s="7" t="s">
+      <c r="I20" s="6" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
+      <c r="A21" s="5">
         <v>42804</v>
       </c>
-      <c r="B21" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" s="4" t="s">
+      <c r="B21" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>43</v>
       </c>
       <c r="E21" t="s">
         <v>5</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="F21" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="G21" s="5">
+      <c r="G21" s="4">
         <v>0.4375</v>
       </c>
-      <c r="H21" s="5">
+      <c r="H21" s="4">
         <v>0.45833333333333331</v>
       </c>
-      <c r="I21" s="7" t="s">
+      <c r="I21" s="6" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="6">
+      <c r="A22" s="5">
         <v>42804</v>
       </c>
-      <c r="B22" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C22" s="4" t="s">
+      <c r="B22" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>43</v>
       </c>
       <c r="E22" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="8" t="s">
+      <c r="F22" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="G22" s="5">
+      <c r="G22" s="4">
         <v>0.47222222222222227</v>
       </c>
-      <c r="H22" s="5">
+      <c r="H22" s="4">
         <v>0.47916666666666669</v>
       </c>
-      <c r="I22" s="7" t="s">
+      <c r="I22" s="6" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="6">
+      <c r="A23" s="5">
         <v>42804</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23" s="4" t="s">
+      <c r="B23" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>43</v>
       </c>
       <c r="E23" t="s">
         <v>5</v>
       </c>
-      <c r="F23" s="8" t="s">
+      <c r="F23" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="G23" s="5">
+      <c r="G23" s="4">
         <v>0.5</v>
       </c>
-      <c r="H23" s="5">
+      <c r="H23" s="4">
         <v>0.54861111111111105</v>
       </c>
-      <c r="I23" s="7" t="s">
+      <c r="I23" s="6" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="6">
+      <c r="A24" s="5">
         <v>42805</v>
       </c>
-      <c r="C24" s="4"/>
+      <c r="C24" s="3"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="6">
+      <c r="A25" s="5">
         <v>42806</v>
       </c>
-      <c r="C25" s="4"/>
+      <c r="C25" s="3"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="6">
+      <c r="A26" s="5">
         <v>42807</v>
       </c>
-      <c r="B26" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C26" s="4" t="s">
+      <c r="B26" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>43</v>
       </c>
       <c r="E26" t="s">
@@ -1299,51 +1340,51 @@
       <c r="F26" t="s">
         <v>87</v>
       </c>
-      <c r="G26" s="5">
+      <c r="G26" s="4">
         <v>0.33680555555555558</v>
       </c>
-      <c r="H26" s="5">
+      <c r="H26" s="4">
         <v>0.37847222222222227</v>
       </c>
-      <c r="I26" s="7" t="s">
+      <c r="I26" s="6" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="6">
+      <c r="A27" s="5">
         <v>42807</v>
       </c>
-      <c r="B27" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D27" s="7"/>
+      <c r="B27" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="6"/>
       <c r="E27" t="s">
         <v>26</v>
       </c>
       <c r="F27" t="s">
         <v>88</v>
       </c>
-      <c r="G27" s="5">
+      <c r="G27" s="4">
         <v>0.38194444444444442</v>
       </c>
-      <c r="H27" s="5">
+      <c r="H27" s="4">
         <v>0.40625</v>
       </c>
-      <c r="I27" s="7" t="s">
+      <c r="I27" s="6" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="6">
+      <c r="A28" s="5">
         <v>42807</v>
       </c>
-      <c r="B28" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C28" s="4" t="s">
+      <c r="B28" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>43</v>
       </c>
       <c r="E28" t="s">
@@ -1352,24 +1393,24 @@
       <c r="F28" t="s">
         <v>89</v>
       </c>
-      <c r="G28" s="5">
+      <c r="G28" s="4">
         <v>0.40625</v>
       </c>
-      <c r="H28" s="5">
+      <c r="H28" s="4">
         <v>0.40972222222222227</v>
       </c>
-      <c r="I28" s="7" t="s">
+      <c r="I28" s="6" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="6">
+      <c r="A29" s="5">
         <v>42807</v>
       </c>
-      <c r="B29" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C29" s="4" t="s">
+      <c r="B29" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>43</v>
       </c>
       <c r="E29" t="s">
@@ -1378,24 +1419,24 @@
       <c r="F29" t="s">
         <v>91</v>
       </c>
-      <c r="G29" s="5">
+      <c r="G29" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="H29" s="5">
+      <c r="H29" s="4">
         <v>0.4375</v>
       </c>
-      <c r="I29" s="7" t="s">
+      <c r="I29" s="6" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="6">
+      <c r="A30" s="5">
         <v>42807</v>
       </c>
-      <c r="B30" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C30" s="4" t="s">
+      <c r="B30" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>43</v>
       </c>
       <c r="E30" t="s">
@@ -1404,54 +1445,296 @@
       <c r="F30" t="s">
         <v>92</v>
       </c>
-      <c r="G30" s="5">
+      <c r="G30" s="4">
         <v>0.44444444444444442</v>
       </c>
-      <c r="H30" s="5">
+      <c r="H30" s="4">
         <v>0.46527777777777773</v>
       </c>
-      <c r="I30" s="7" t="s">
+      <c r="I30" s="6" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="6">
+      <c r="A31" s="5">
+        <v>42807</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" t="s">
+        <v>26</v>
+      </c>
+      <c r="F31" t="s">
+        <v>93</v>
+      </c>
+      <c r="G31" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="H31" s="4">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>42807</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E32" t="s">
+        <v>5</v>
+      </c>
+      <c r="F32" t="s">
+        <v>94</v>
+      </c>
+      <c r="G32" s="4">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="H32" s="4">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>42807</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" t="s">
+        <v>100</v>
+      </c>
+      <c r="G33" s="4">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="H33" s="4">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
         <v>42808</v>
       </c>
-      <c r="C31" s="4"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="6">
+      <c r="B34" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E34" t="s">
+        <v>3</v>
+      </c>
+      <c r="F34" t="s">
+        <v>97</v>
+      </c>
+      <c r="G34" s="4">
+        <v>0.34375</v>
+      </c>
+      <c r="H34" s="4">
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <v>42808</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E35" t="s">
+        <v>3</v>
+      </c>
+      <c r="F35" t="s">
+        <v>98</v>
+      </c>
+      <c r="G35" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H35" s="4">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="I35" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="5">
+        <v>42808</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E36" t="s">
+        <v>26</v>
+      </c>
+      <c r="F36" t="s">
+        <v>101</v>
+      </c>
+      <c r="G36" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="H36" s="4">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="I36" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="5">
+        <v>42808</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E37" t="s">
+        <v>26</v>
+      </c>
+      <c r="F37" t="s">
+        <v>102</v>
+      </c>
+      <c r="G37" s="4">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="H37" s="4">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="I37" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="5">
+        <v>42808</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E38" t="s">
+        <v>26</v>
+      </c>
+      <c r="F38" t="s">
+        <v>103</v>
+      </c>
+      <c r="G38" s="4">
+        <v>0.58680555555555558</v>
+      </c>
+      <c r="H38" s="4">
+        <v>0.60763888888888895</v>
+      </c>
+      <c r="I38" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="5">
+        <v>42808</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E39" t="s">
+        <v>26</v>
+      </c>
+      <c r="F39" t="s">
+        <v>104</v>
+      </c>
+      <c r="G39" s="4">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="H39" s="4">
+        <v>0.62152777777777779</v>
+      </c>
+      <c r="I39" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="5">
+        <v>42808</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E40" t="s">
+        <v>26</v>
+      </c>
+      <c r="F40" t="s">
+        <v>105</v>
+      </c>
+      <c r="G40" s="4">
+        <v>0.62152777777777779</v>
+      </c>
+      <c r="H40" s="4">
+        <v>0.63194444444444442</v>
+      </c>
+      <c r="I40" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="5">
         <v>42809</v>
       </c>
-      <c r="C32" s="4"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="6">
+      <c r="C41" s="3"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="5">
         <v>42810</v>
       </c>
-      <c r="C33" s="4"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="C34" s="4"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="C35" s="4"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E116">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E122">
       <formula1>GyldigeRoller</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C35">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C41">
       <formula1>Deltagere</formula1>
     </dataValidation>
   </dataValidations>
@@ -1473,7 +1756,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Har tilføjet implements til NormalspaendingImpl - importeret kalsser til OC5Test
</commit_message>
<xml_diff>
--- a/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering i PTE projektet - Nada Omer.xlsx
+++ b/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering i PTE projektet - Nada Omer.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="118">
   <si>
     <t>Business-Process Analyst</t>
   </si>
@@ -333,9 +333,6 @@
     <t>1 time : 25 min.</t>
   </si>
   <si>
-    <t>Implementerer OC4</t>
-  </si>
-  <si>
     <t>Krydstjeck for UC7</t>
   </si>
   <si>
@@ -352,6 +349,42 @@
   </si>
   <si>
     <t>0 time : 15 min.</t>
+  </si>
+  <si>
+    <t>Review OC7</t>
+  </si>
+  <si>
+    <t>Implementer OC4</t>
+  </si>
+  <si>
+    <t>Implementer Junit test til OC5</t>
+  </si>
+  <si>
+    <t>Prøver at implemente Junit test til OC7, men Testsutie var indvalid.</t>
+  </si>
+  <si>
+    <t>SD og DCD for OC7</t>
+  </si>
+  <si>
+    <t>1 time : 20 min.</t>
+  </si>
+  <si>
+    <t>Implementer OC5</t>
+  </si>
+  <si>
+    <t>Prøver at implemente OC5, men Design var indvalid.</t>
+  </si>
+  <si>
+    <t>Implementer OC7</t>
+  </si>
+  <si>
+    <t>Implementer  Junit test til OC7</t>
+  </si>
+  <si>
+    <t>0 time : 50 min.</t>
+  </si>
+  <si>
+    <t>0 time : 40 min.</t>
   </si>
 </sst>
 </file>
@@ -734,10 +767,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K42"/>
+  <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="I50" sqref="I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,7 +780,7 @@
     <col min="3" max="3" width="17.85546875" customWidth="1"/>
     <col min="4" max="4" width="7.140625" customWidth="1"/>
     <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="48.140625" customWidth="1"/>
+    <col min="6" max="6" width="59.5703125" customWidth="1"/>
     <col min="9" max="9" width="24.5703125" customWidth="1"/>
     <col min="11" max="11" width="31.85546875" customWidth="1"/>
   </cols>
@@ -1521,7 +1554,7 @@
         <v>9</v>
       </c>
       <c r="F33" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="G33" s="4">
         <v>0.59722222222222221</v>
@@ -1599,7 +1632,7 @@
         <v>26</v>
       </c>
       <c r="F36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G36" s="4">
         <v>0.5</v>
@@ -1625,7 +1658,7 @@
         <v>26</v>
       </c>
       <c r="F37" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G37" s="4">
         <v>0.54166666666666663</v>
@@ -1651,7 +1684,7 @@
         <v>26</v>
       </c>
       <c r="F38" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G38" s="4">
         <v>0.58680555555555558</v>
@@ -1677,7 +1710,7 @@
         <v>26</v>
       </c>
       <c r="F39" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G39" s="4">
         <v>0.61458333333333337</v>
@@ -1703,7 +1736,7 @@
         <v>26</v>
       </c>
       <c r="F40" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G40" s="4">
         <v>0.62152777777777779</v>
@@ -1712,18 +1745,235 @@
         <v>0.63194444444444442</v>
       </c>
       <c r="I40" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>42809</v>
       </c>
-      <c r="C41" s="3"/>
+      <c r="B41" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E41" t="s">
+        <v>26</v>
+      </c>
+      <c r="F41" t="s">
+        <v>106</v>
+      </c>
+      <c r="G41" s="4">
+        <v>0.35069444444444442</v>
+      </c>
+      <c r="H41" s="4">
+        <v>0.375</v>
+      </c>
+      <c r="I41" s="6" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
+        <v>42809</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E42" t="s">
+        <v>5</v>
+      </c>
+      <c r="F42" t="s">
+        <v>110</v>
+      </c>
+      <c r="G42" s="4">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="H42" s="4">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="I42" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="5">
+        <v>42809</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E43" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" t="s">
+        <v>108</v>
+      </c>
+      <c r="G43" s="4">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="H43" s="4">
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="I43" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="5">
+        <v>42809</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E44" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44" t="s">
+        <v>109</v>
+      </c>
+      <c r="G44" s="4">
+        <v>0.53125</v>
+      </c>
+      <c r="H44" s="4">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="I44" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="5">
+        <v>42809</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E45" t="s">
+        <v>9</v>
+      </c>
+      <c r="F45" t="s">
+        <v>113</v>
+      </c>
+      <c r="G45" s="4">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="H45" s="4">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="I45" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="5">
+        <v>42809</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E46" t="s">
+        <v>9</v>
+      </c>
+      <c r="F46" t="s">
+        <v>114</v>
+      </c>
+      <c r="G46" s="4">
+        <v>0.60069444444444442</v>
+      </c>
+      <c r="H46" s="4">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="I46" s="6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="5">
         <v>42810</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E47" t="s">
+        <v>9</v>
+      </c>
+      <c r="F47" t="s">
+        <v>114</v>
+      </c>
+      <c r="G47" s="4">
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="H47" s="4">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="I47" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="5">
+        <v>42810</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E48" t="s">
+        <v>9</v>
+      </c>
+      <c r="F48" t="s">
+        <v>112</v>
+      </c>
+      <c r="G48" s="4">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="H48" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="I48" s="6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="5">
+        <v>42810</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E49" t="s">
+        <v>9</v>
+      </c>
+      <c r="F49" t="s">
+        <v>115</v>
+      </c>
+      <c r="G49" s="4">
+        <v>0.4236111111111111</v>
       </c>
     </row>
   </sheetData>
@@ -1731,11 +1981,11 @@
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E122">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C49">
+      <formula1>Deltagere</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E124">
       <formula1>GyldigeRoller</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C41">
-      <formula1>Deltagere</formula1>
     </dataValidation>
   </dataValidations>
   <printOptions headings="1"/>

</xml_diff>

<commit_message>
Implementer  Junit test til OC7 + setFnNewton + setFtNewton
</commit_message>
<xml_diff>
--- a/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering i PTE projektet - Nada Omer.xlsx
+++ b/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering i PTE projektet - Nada Omer.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="119">
   <si>
     <t>Business-Process Analyst</t>
   </si>
@@ -378,13 +378,16 @@
     <t>Implementer OC7</t>
   </si>
   <si>
-    <t>Implementer  Junit test til OC7</t>
-  </si>
-  <si>
     <t>0 time : 50 min.</t>
   </si>
   <si>
     <t>0 time : 40 min.</t>
+  </si>
+  <si>
+    <t>1 time : 50 min.</t>
+  </si>
+  <si>
+    <t>Implementer  Junit test til OC7 + setFnNewton + setFtNewton</t>
   </si>
 </sst>
 </file>
@@ -769,8 +772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="I50" sqref="I50"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1901,7 +1904,7 @@
         <v>0.63541666666666663</v>
       </c>
       <c r="I46" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -1953,10 +1956,10 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="I48" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>42810</v>
       </c>
@@ -1970,10 +1973,16 @@
         <v>9</v>
       </c>
       <c r="F49" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="G49" s="4">
         <v>0.4236111111111111</v>
+      </c>
+      <c r="H49" s="4">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="I49" s="6" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Prøver at løse problemet med at committe GUI design
</commit_message>
<xml_diff>
--- a/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering i PTE projektet - Nada Omer.xlsx
+++ b/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering i PTE projektet - Nada Omer.xlsx
@@ -772,8 +772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Vægt felt håndterer komma nu
</commit_message>
<xml_diff>
--- a/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering i PTE projektet - Nada Omer.xlsx
+++ b/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering i PTE projektet - Nada Omer.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="127">
   <si>
     <t>Business-Process Analyst</t>
   </si>
@@ -388,6 +388,30 @@
   </si>
   <si>
     <t>Implementer  Junit test til OC7 + setFnNewton + setFtNewton</t>
+  </si>
+  <si>
+    <t>Implementer  Junit test til OC5</t>
+  </si>
+  <si>
+    <t>GUI Design</t>
+  </si>
+  <si>
+    <t>Bruger Test</t>
+  </si>
+  <si>
+    <t>Review OC15</t>
+  </si>
+  <si>
+    <t>GUI Design - SigmaN + rettelser til udskrivning af mellemregninger</t>
+  </si>
+  <si>
+    <t>7 time : 55 min.</t>
+  </si>
+  <si>
+    <t>2 time : 00 min.</t>
+  </si>
+  <si>
+    <t>2 time : 30 min.</t>
   </si>
 </sst>
 </file>
@@ -770,10 +794,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K49"/>
+  <dimension ref="A1:K57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="I57" sqref="I57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1911,31 +1935,15 @@
       <c r="A47" s="5">
         <v>42810</v>
       </c>
-      <c r="B47" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E47" t="s">
-        <v>9</v>
-      </c>
-      <c r="F47" t="s">
-        <v>114</v>
-      </c>
-      <c r="G47" s="4">
-        <v>0.33680555555555558</v>
-      </c>
-      <c r="H47" s="4">
-        <v>0.38541666666666669</v>
-      </c>
-      <c r="I47" s="6" t="s">
-        <v>86</v>
-      </c>
+      <c r="B47" s="6"/>
+      <c r="C47" s="3"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="6"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
-        <v>42810</v>
+        <v>42811</v>
       </c>
       <c r="B48" s="6" t="s">
         <v>55</v>
@@ -1947,21 +1955,21 @@
         <v>9</v>
       </c>
       <c r="F48" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="G48" s="4">
-        <v>0.3888888888888889</v>
+        <v>0.33680555555555558</v>
       </c>
       <c r="H48" s="4">
-        <v>0.41666666666666669</v>
+        <v>0.38541666666666669</v>
       </c>
       <c r="I48" s="6" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
-        <v>42810</v>
+        <v>42811</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>55</v>
@@ -1973,16 +1981,190 @@
         <v>9</v>
       </c>
       <c r="F49" t="s">
+        <v>112</v>
+      </c>
+      <c r="G49" s="4">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="H49" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="I49" s="6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="5">
+        <v>42811</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E50" t="s">
+        <v>9</v>
+      </c>
+      <c r="F50" t="s">
         <v>118</v>
       </c>
-      <c r="G49" s="4">
+      <c r="G50" s="4">
         <v>0.4236111111111111</v>
       </c>
-      <c r="H49" s="4">
+      <c r="H50" s="4">
         <v>0.52083333333333337</v>
       </c>
-      <c r="I49" s="6" t="s">
+      <c r="I50" s="6" t="s">
         <v>117</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="5">
+        <v>42811</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E51" t="s">
+        <v>9</v>
+      </c>
+      <c r="F51" t="s">
+        <v>119</v>
+      </c>
+      <c r="G51" s="4">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="H51" s="4">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="I51" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="5">
+        <v>42812</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52" s="3"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="5">
+        <v>42813</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C53" s="3"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="5">
+        <v>42814</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E54" t="s">
+        <v>9</v>
+      </c>
+      <c r="F54" t="s">
+        <v>120</v>
+      </c>
+      <c r="G54" s="4">
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="H54" s="4">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="I54" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="5">
+        <v>42815</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E55" t="s">
+        <v>19</v>
+      </c>
+      <c r="F55" t="s">
+        <v>121</v>
+      </c>
+      <c r="G55" s="4">
+        <v>0.34375</v>
+      </c>
+      <c r="H55" s="4">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="I55" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="5">
+        <v>42815</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E56" t="s">
+        <v>26</v>
+      </c>
+      <c r="F56" t="s">
+        <v>122</v>
+      </c>
+      <c r="G56" s="4">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="H56" s="4">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="I56" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="5">
+        <v>42815</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E57" t="s">
+        <v>9</v>
+      </c>
+      <c r="F57" t="s">
+        <v>123</v>
+      </c>
+      <c r="G57" s="4">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="H57" s="4">
+        <v>0.5625</v>
+      </c>
+      <c r="I57" s="6" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1990,10 +2172,10 @@
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C49">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C57">
       <formula1>Deltagere</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E124">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E126">
       <formula1>GyldigeRoller</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
SigmaB er rettet til store s
</commit_message>
<xml_diff>
--- a/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering i PTE projektet - Nada Omer.xlsx
+++ b/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering i PTE projektet - Nada Omer.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="133">
   <si>
     <t>Business-Process Analyst</t>
   </si>
@@ -412,6 +412,24 @@
   </si>
   <si>
     <t>2 time : 30 min.</t>
+  </si>
+  <si>
+    <t>GUI programmering</t>
+  </si>
+  <si>
+    <t>8 time : 50 min.</t>
+  </si>
+  <si>
+    <t>7 time : 10 min.</t>
+  </si>
+  <si>
+    <t>GUI programmering + Logic for mellemregniner formler</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Logic for mellemregniner formler</t>
+  </si>
+  <si>
+    <t>5 time : 00 min.</t>
   </si>
 </sst>
 </file>
@@ -794,10 +812,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K57"/>
+  <dimension ref="A1:K60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="I57" sqref="I57"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2167,12 +2185,90 @@
         <v>126</v>
       </c>
     </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="5">
+        <v>42816</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E58" t="s">
+        <v>9</v>
+      </c>
+      <c r="F58" t="s">
+        <v>127</v>
+      </c>
+      <c r="G58" s="4">
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="H58" s="4">
+        <v>0.70486111111111116</v>
+      </c>
+      <c r="I58" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="5">
+        <v>42817</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E59" t="s">
+        <v>9</v>
+      </c>
+      <c r="F59" t="s">
+        <v>130</v>
+      </c>
+      <c r="G59" s="4">
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="H59" s="4">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="I59" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="5">
+        <v>42818</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E60" t="s">
+        <v>9</v>
+      </c>
+      <c r="F60" t="s">
+        <v>131</v>
+      </c>
+      <c r="G60" s="4">
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="H60" s="4">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="I60" s="6" t="s">
+        <v>132</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C57">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C60">
       <formula1>Deltagere</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E126">

</xml_diff>